<commit_message>
Added most of densenet results
</commit_message>
<xml_diff>
--- a/codecarbon/results.xlsx
+++ b/codecarbon/results.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:B42"/>
+  <dimension ref="A2:B112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,7 +557,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15"/>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
@@ -694,10 +693,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr"/>
-      <c r="B29" t="inlineStr"/>
-    </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
@@ -831,6 +826,691 @@
         </is>
       </c>
       <c r="B42" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>DenseNet</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>CIFAR10</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Evaluation Framework</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>codecarbon</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Total Energy (kWh)</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.007889708648527477</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Total CO2 Emissions (kgCO2e)</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.003665334359850078</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CPU Energy</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.003676336044128321</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>GPU Energy</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.003868527261486</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Training Time (minutes)</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>3.529349748293559</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0.4979</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0.5076567591666675</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0.4979</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>F1</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.4938883820971905</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Number of Epochs</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>DenseNet</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>CIFAR10</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Evaluation Framework</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>codecarbon</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Total Energy (kWh)</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>0.01376071803926909</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Total CO2 Emissions (kgCO2e)</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0.006392838429459039</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>CPU Energy</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0.006502480990958347</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>GPU Energy</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0.006648244763035999</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Training Time (minutes)</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>6.24258105357488</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.6074000000000001</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.60533981406285</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0.6074000000000001</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>F1</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0.6015483504098486</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Number of Epochs</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>DenseNet</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>CIFAR10</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Evaluation Framework</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>codecarbon</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Total Energy (kWh)</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0.01381779868302146</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Total CO2 Emissions (kgCO2e)</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0.00641935647393296</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>CPU Energy</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.006506989855818876</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>GPU Energy</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0.006700420915888</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Training Time (minutes)</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>6.246892023086548</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>0.8308</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>0.8312846509078877</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>0.8308</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>F1</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>0.8308816365228535</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Number of Epochs</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85"/>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>DenseNet</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>MNIST</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Evaluation Framework</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>codecarbon</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Total Energy (kWh)</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>0.02369511978299916</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Total CO2 Emissions (kgCO2e)</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>0.01100807907749544</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>CPU Energy</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>0.01102109265664694</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>GPU Energy</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>0.01164026486776</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Training Time (minutes)</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>10.58042073647181</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>0.991</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>0.9910263475630446</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>0.991</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>F1</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>0.9909997736228469</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Number of Epochs</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr"/>
+      <c r="B99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>DenseNet</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>MNIST</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Evaluation Framework</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>codecarbon</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Total Energy (kWh)</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>0.2368809560385094</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Total CO2 Emissions (kgCO2e)</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>0.110048158435373</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>CPU Energy</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>0.1101841889024743</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>GPU Energy</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>0.116361546978052</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Training Time (minutes)</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>105.777428428332</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>0.9957</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>0.9957108101984441</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>0.9957</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>F1</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>0.9956985806654162</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Number of Epochs</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>